<commit_message>
Duplication check in registration
</commit_message>
<xml_diff>
--- a/Files/IKSANA_API_TEST_SCRIPTS_v0.1.xlsx
+++ b/Files/IKSANA_API_TEST_SCRIPTS_v0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" activeTab="2"/>
+    <workbookView windowWidth="19200" windowHeight="6080" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="58">
   <si>
     <t>S.NO</t>
   </si>
@@ -162,7 +162,67 @@
     <t>Registration with Duplicate Email and Phone without caregiver</t>
   </si>
   <si>
+    <t>Verify the API response status and validation of duplicate phone number.</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>The response should contain "Already exist" message</t>
+  </si>
+  <si>
+    <t>The response contain expected message.</t>
+  </si>
+  <si>
     <t>Registration_TC_08</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of duplicate email.</t>
+  </si>
+  <si>
+    <t>Registration_TC_09</t>
+  </si>
+  <si>
+    <t>Registration with Duplicate Email and Phone with caregiver</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of duplicate phone number in User Data and Caregiver</t>
+  </si>
+  <si>
+    <t>The response should contain "1111" code and "Already exist" message</t>
+  </si>
+  <si>
+    <t>The response contain expected code and message.</t>
+  </si>
+  <si>
+    <t>Registration_TC_10</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of duplicate email in User Data and Caregiver</t>
+  </si>
+  <si>
+    <t>Registration_TC_11</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of duplicate phone in Caregiver that already exists in DB</t>
+  </si>
+  <si>
+    <t>Registration_TC_12</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of duplicate email in Caregiver that already exists in DB</t>
+  </si>
+  <si>
+    <t>Registration_TC_13</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of duplicate phone among multiple Caregivers in same request</t>
+  </si>
+  <si>
+    <t>Registration_TC_14</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of duplicate email among multiple Caregivers in same request</t>
   </si>
 </sst>
 </file>
@@ -872,7 +932,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -924,6 +984,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -932,9 +1004,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1503,8 +1572,8 @@
   <sheetPr/>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1588,10 +1657,10 @@
       <c r="I2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="23" t="s">
         <v>21</v>
       </c>
       <c r="L2" s="5" t="s">
@@ -1624,10 +1693,10 @@
       <c r="I3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="23" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
@@ -1660,10 +1729,10 @@
       <c r="I4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="22" t="s">
         <v>30</v>
       </c>
       <c r="L4" s="5" t="s">
@@ -1698,10 +1767,10 @@
       <c r="I5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="23" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="5" t="s">
@@ -1734,10 +1803,10 @@
       <c r="I6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="23" t="s">
         <v>26</v>
       </c>
       <c r="L6" s="5" t="s">
@@ -1770,10 +1839,10 @@
       <c r="I7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="22" t="s">
         <v>30</v>
       </c>
       <c r="L7" s="5" t="s">
@@ -1793,337 +1862,504 @@
       <c r="D8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="5"/>
+      <c r="E8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:12">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="5"/>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:12">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="5"/>
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" ht="30" customHeight="1" spans="1:12">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="5"/>
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" ht="30" customHeight="1" spans="1:12">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="5"/>
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" ht="30" customHeight="1" spans="1:12">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="5"/>
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" ht="30" customHeight="1" spans="1:12">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="5"/>
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" ht="30" customHeight="1" spans="1:12">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="5"/>
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" ht="30" customHeight="1" spans="1:12">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
       <c r="L16" s="5"/>
     </row>
     <row r="17" ht="30" customHeight="1" spans="1:12">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
       <c r="L17" s="5"/>
     </row>
     <row r="18" ht="30" customHeight="1" spans="1:12">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
       <c r="L18" s="5"/>
     </row>
     <row r="19" ht="30" customHeight="1" spans="1:12">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
       <c r="L19" s="5"/>
     </row>
     <row r="20" ht="30" customHeight="1" spans="1:12">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
       <c r="L20" s="5"/>
     </row>
     <row r="21" ht="30" customHeight="1" spans="1:12">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
       <c r="L21" s="5"/>
     </row>
     <row r="22" ht="30" customHeight="1" spans="1:12">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" ht="30" customHeight="1" spans="1:12">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
       <c r="L23" s="5"/>
     </row>
     <row r="24" ht="30" customHeight="1" spans="1:12">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
       <c r="L24" s="5"/>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:12">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
       <c r="L25" s="5"/>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:12">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
       <c r="L26" s="5"/>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:12">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
       <c r="L27" s="5"/>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:12">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
       <c r="L28" s="5"/>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:12">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
       <c r="L29" s="5"/>
     </row>
     <row r="30" ht="30" customHeight="1" spans="7:12">
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
       <c r="L30" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D15"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H8 H9:H15">
       <formula1>"GET,POST,PUT,DELETE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I8 I9:I15">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L8 L9:L15">
       <formula1>"Pass,Fail,Hold"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Login API Automation Iniated
</commit_message>
<xml_diff>
--- a/Files/IKSANA_API_TEST_SCRIPTS_v0.1.xlsx
+++ b/Files/IKSANA_API_TEST_SCRIPTS_v0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6080" activeTab="2"/>
+    <workbookView windowWidth="19200" windowHeight="6080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="84">
   <si>
     <t>S.NO</t>
   </si>
@@ -65,6 +65,65 @@
   </si>
   <si>
     <t>Test status</t>
+  </si>
+  <si>
+    <t>Login_TC_1</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Login with Registered mobile number</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/user-registration</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status, Response code and message.</t>
+  </si>
+  <si>
+    <t>validate-phone-number</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>HTTP status code should be 200 and The response should contain "0000" code and "Otp Genereated Successfully" message</t>
+  </si>
+  <si>
+    <t>The response contain expected fields.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Login_TC_2</t>
+  </si>
+  <si>
+    <t>Login with UnRegistered mobile number</t>
   </si>
   <si>
     <t>Registration_TC_01</t>
@@ -108,18 +167,12 @@
     <t>POST</t>
   </si>
   <si>
-    <t>Positive</t>
-  </si>
-  <si>
     <t>HTTP status code should be 200 OK.</t>
   </si>
   <si>
     <t>200 OK</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>Registration_TC_02</t>
   </si>
   <si>
@@ -141,9 +194,6 @@
     <t>The response should contain expected fields.</t>
   </si>
   <si>
-    <t>The response contain expected fields.</t>
-  </si>
-  <si>
     <t>Registration_TC_04</t>
   </si>
   <si>
@@ -223,6 +273,54 @@
   </si>
   <si>
     <t>Verify the API response status and validation of duplicate email among multiple Caregivers in same request</t>
+  </si>
+  <si>
+    <t>Registration_TC_15</t>
+  </si>
+  <si>
+    <t>Registration with More than 4 FamilyMembers</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for More than 4 Caregivers in the request</t>
+  </si>
+  <si>
+    <t>The response should contain "1111" code and "You can add up to 4 members only." message</t>
+  </si>
+  <si>
+    <t>Registration_TC_16</t>
+  </si>
+  <si>
+    <t>Registration with Null values without caregiver</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of phone number field upon null values.</t>
+  </si>
+  <si>
+    <t>The response should contain "1111" code and "Data should not be empty" message</t>
+  </si>
+  <si>
+    <t>Registration_TC_17</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of email field upon null values.</t>
+  </si>
+  <si>
+    <t>Registration_TC_18</t>
+  </si>
+  <si>
+    <t>Registration with Null values with caregiver</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of phone number field upon null values on caregiver.</t>
+  </si>
+  <si>
+    <t>Registration_TC_19</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of email field upon null values on caregiver.</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -235,7 +333,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +376,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -802,137 +907,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -984,26 +1089,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1554,14 +1665,176 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.63636363636364" customWidth="1"/>
+    <col min="2" max="2" width="18.9090909090909" customWidth="1"/>
+    <col min="3" max="3" width="17.6363636363636" customWidth="1"/>
+    <col min="4" max="4" width="26.2727272727273" customWidth="1"/>
+    <col min="5" max="5" width="32.7272727272727" customWidth="1"/>
+    <col min="6" max="6" width="35.2727272727273" customWidth="1"/>
+    <col min="7" max="7" width="22.3636363636364" customWidth="1"/>
+    <col min="8" max="8" width="11.8181818181818" customWidth="1"/>
+    <col min="9" max="9" width="15.2727272727273" customWidth="1"/>
+    <col min="10" max="10" width="31.1818181818182" customWidth="1"/>
+    <col min="11" max="11" width="22.8181818181818" customWidth="1"/>
+    <col min="12" max="12" width="13.2727272727273" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1" spans="1:12">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:12">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:12">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1"/>
+    <row r="5" ht="30" customHeight="1"/>
+    <row r="6" ht="30" customHeight="1"/>
+    <row r="7" ht="30" customHeight="1"/>
+    <row r="8" ht="30" customHeight="1"/>
+    <row r="9" ht="30" customHeight="1"/>
+    <row r="10" ht="30" customHeight="1"/>
+    <row r="11" ht="30" customHeight="1"/>
+    <row r="12" ht="30" customHeight="1"/>
+    <row r="13" ht="30" customHeight="1"/>
+    <row r="14" ht="30" customHeight="1"/>
+    <row r="15" ht="30" customHeight="1"/>
+    <row r="16" ht="30" customHeight="1"/>
+    <row r="17" ht="30" customHeight="1"/>
+    <row r="18" ht="30" customHeight="1"/>
+    <row r="19" ht="30" customHeight="1"/>
+    <row r="20" ht="30" customHeight="1"/>
+    <row r="21" ht="30" customHeight="1"/>
+    <row r="22" ht="30" customHeight="1"/>
+    <row r="23" ht="30" customHeight="1"/>
+    <row r="24" ht="30" customHeight="1"/>
+    <row r="25" ht="30" customHeight="1"/>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1 I2:I3">
+      <formula1>"Positive,Negative"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1 L2:L3">
+      <formula1>"Pass,Fail,Hold"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3">
+      <formula1>"GET,POST,PUT,DELETE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1572,8 +1845,8 @@
   <sheetPr/>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1634,34 +1907,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>21</v>
+      <c r="J2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>22</v>
@@ -1672,32 +1945,32 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="23" t="s">
-        <v>26</v>
+      <c r="J3" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>22</v>
@@ -1708,32 +1981,32 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>30</v>
+      <c r="J4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>22</v>
@@ -1744,34 +2017,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>21</v>
+      <c r="J5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>22</v>
@@ -1782,32 +2055,32 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>26</v>
+      <c r="J6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>22</v>
@@ -1818,32 +2091,32 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>30</v>
+      <c r="J7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>22</v>
@@ -1854,34 +2127,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>22</v>
@@ -1892,32 +2165,32 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>22</v>
@@ -1928,34 +2201,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>44</v>
+        <v>26</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>45</v>
+        <v>28</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>47</v>
+        <v>56</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>22</v>
@@ -1966,32 +2239,32 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="J11" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>47</v>
+        <v>56</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>22</v>
@@ -2002,32 +2275,32 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="19"/>
+        <v>26</v>
+      </c>
+      <c r="D12" s="14"/>
       <c r="E12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>51</v>
+        <v>28</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>47</v>
+        <v>56</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>22</v>
@@ -2038,32 +2311,32 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="19"/>
+        <v>26</v>
+      </c>
+      <c r="D13" s="14"/>
       <c r="E13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>53</v>
+        <v>28</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>47</v>
+        <v>56</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>22</v>
@@ -2074,32 +2347,32 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="19"/>
+        <v>26</v>
+      </c>
+      <c r="D14" s="14"/>
       <c r="E14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>55</v>
+        <v>28</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>47</v>
+        <v>56</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>22</v>
@@ -2110,106 +2383,222 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="18" t="s">
+      <c r="K15" s="18" t="s">
         <v>57</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>47</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" ht="30" customHeight="1" spans="1:12">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="5"/>
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" ht="30" customHeight="1" spans="1:12">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="5"/>
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" ht="30" customHeight="1" spans="1:12">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="5"/>
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" ht="30" customHeight="1" spans="1:12">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="5"/>
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" ht="30" customHeight="1" spans="1:12">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="5"/>
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L20" s="23" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="21" ht="30" customHeight="1" spans="1:12">
       <c r="A21" s="21"/>
@@ -2346,20 +2735,22 @@
       <c r="L30" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D10:D15"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H8 H9:H15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H20">
       <formula1>"GET,POST,PUT,DELETE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I8 I9:I15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I20">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L8 L9:L15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L20">
       <formula1>"Pass,Fail,Hold"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
validation of OTP in login
</commit_message>
<xml_diff>
--- a/Files/IKSANA_API_TEST_SCRIPTS_v0.1.xlsx
+++ b/Files/IKSANA_API_TEST_SCRIPTS_v0.1.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="135">
   <si>
     <t>S.NO</t>
   </si>
@@ -73,7 +73,7 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Login with Registered mobile number</t>
+    <t>phoneNoVerificationSuccess</t>
   </si>
   <si>
     <r>
@@ -95,11 +95,11 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> http://135.181.193.65:8080/user-registration</t>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=+91&amp;phoneNo=6554433444&amp;login=false&amp;hashValue=5CH1ajIvhkB</t>
     </r>
   </si>
   <si>
-    <t>Verify the API response status, Response code and message.</t>
+    <t>Verify the API response status, Response code and message for Registered Phone number</t>
   </si>
   <si>
     <t>validate-phone-number</t>
@@ -123,7 +123,416 @@
     <t>Login_TC_2</t>
   </si>
   <si>
-    <t>Login with UnRegistered mobile number</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=+91&amp;phoneNo=8756453782&amp;login=false&amp;hashValue=5CH1ajIvhkB</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Verify the API response status, Response code and message for </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UnR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>egistered Phone number.</t>
+    </r>
+  </si>
+  <si>
+    <t>Login_TC_3</t>
+  </si>
+  <si>
+    <t>phoneNoValidationCheck</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=+91&amp;phoneNo=&amp;login=false&amp;hashValue=5CH1ajIvhkB</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for phone number field in the Blank phone number scenario</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>HTTP status code should be 200 and The response should contain "1111" code and "Please enter valid phone number" message</t>
+  </si>
+  <si>
+    <t>Login_TC_4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=+91&amp;phoneNo=24556343&amp;login=false&amp;hashValue=5CH1ajIvhkB</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for phone number field Phone number with less than 10 digits.</t>
+  </si>
+  <si>
+    <t>Login_TC_5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=+91&amp;phoneNo=3756756789&amp;login=false&amp;hashValue=5CH1ajIvhkB</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for phone number field Phone number first digit is &lt;=4 and 10 digit</t>
+  </si>
+  <si>
+    <t>Login_TC_6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=+91&amp;phoneNo=abc@123!&amp;login=false&amp;hashValue=5CH1ajIvhkB</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for phone number field Phone number with characters or special symbols</t>
+  </si>
+  <si>
+    <t>Login_TC_7</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=&amp;phoneNo=abc@123!&amp;login=false&amp;hashValue=5CH1ajIvhkB</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for CountryCode field with Blank country code</t>
+  </si>
+  <si>
+    <t>The response not as Expected</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Login_TC_8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=+1&amp;phoneNo=abc@123!&amp;login=false&amp;hashValue=5CH1ajIvhkB</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for CountryCode field with Different valid region</t>
+  </si>
+  <si>
+    <t>Login_TC_9</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=91&amp;phoneNo=abc@123!&amp;login=false&amp;hashValue=5CH1ajIvhkB</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for CountryCode field with Missing '+' sign</t>
+  </si>
+  <si>
+    <t>Login_TC_10</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=@#$&amp;phoneNo=abc@123!&amp;login=false&amp;hashValue=5CH1ajIvhkB</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for CountryCode field with Invalid special characters</t>
+  </si>
+  <si>
+    <t>Login_TC_11</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/validate-phone-number?countryCode=@#$&amp;phoneNo=abc@123!&amp;login=false&amp;hashValue=</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for Hash Value field with Blank Hash Value</t>
+  </si>
+  <si>
+    <t>Login_TC_12</t>
+  </si>
+  <si>
+    <t>LoginSuccessWithReqPhoneNO</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/login-with-otp</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for Registered User</t>
+  </si>
+  <si>
+    <t>login-with-otp</t>
+  </si>
+  <si>
+    <t>HTTP status code should be 200 and The response should contain "0000" code and "Login Successfull" message</t>
+  </si>
+  <si>
+    <t>Login_TC_13</t>
+  </si>
+  <si>
+    <t>LoginSuccessWithUnReqPhoneNO</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for UnRegistered User</t>
+  </si>
+  <si>
+    <t>HTTP status code should be 200 and The response should contain "1313" code and "User Not registered" message</t>
+  </si>
+  <si>
+    <t>Login_TC_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LogInValidationCheck</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for wrong phone and correct OTP in OTP verification.</t>
+  </si>
+  <si>
+    <t>HTTP status code should be 200 and The response should contain "1111" code and "Please verfify your data" message.</t>
+  </si>
+  <si>
+    <t>Login_TC_15</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for wrong OTP in OTP verification.</t>
+  </si>
+  <si>
+    <t>HTTP status code should be 200 and The response should contain "1111" code and "Enter Valid OTP" message.</t>
+  </si>
+  <si>
+    <t>Login_TC_16</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for Expired OTP in OTP verification.</t>
+  </si>
+  <si>
+    <t>HTTP status code should be 200 and The response should contain "1111" code and "OTP Expired" message.</t>
   </si>
   <si>
     <t>Registration_TC_01</t>
@@ -215,9 +624,6 @@
     <t>Verify the API response status and validation of duplicate phone number.</t>
   </si>
   <si>
-    <t>Negative</t>
-  </si>
-  <si>
     <t>The response should contain "Already exist" message</t>
   </si>
   <si>
@@ -318,9 +724,6 @@
   </si>
   <si>
     <t>Verify the API response status and validation of email field upon null values on caregiver.</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -333,7 +736,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +929,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -729,7 +1140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -784,6 +1195,43 @@
         <color auto="1"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -913,7 +1361,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -925,34 +1373,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1037,7 +1485,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1107,14 +1555,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1667,8 +2142,8 @@
   <sheetPr/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1676,7 +2151,7 @@
     <col min="1" max="1" width="5.63636363636364" customWidth="1"/>
     <col min="2" max="2" width="18.9090909090909" customWidth="1"/>
     <col min="3" max="3" width="17.6363636363636" customWidth="1"/>
-    <col min="4" max="4" width="26.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="28.9090909090909" customWidth="1"/>
     <col min="5" max="5" width="32.7272727272727" customWidth="1"/>
     <col min="6" max="6" width="35.2727272727273" customWidth="1"/>
     <col min="7" max="7" width="22.3636363636364" customWidth="1"/>
@@ -1694,7 +2169,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -1703,7 +2178,7 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -1735,7 +2210,7 @@
       <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -1764,57 +2239,553 @@
       </c>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:12">
-      <c r="A3" s="5">
+      <c r="A3" s="25">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:12">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:12">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" ht="30" customHeight="1" spans="1:12">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:12">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1" spans="1:12">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1" spans="1:12">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="1:12">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" ht="30" customHeight="1" spans="1:12">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" ht="30" customHeight="1" spans="1:12">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" ht="30" customHeight="1" spans="1:12">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" ht="30" customHeight="1" spans="1:12">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" ht="30" customHeight="1" spans="1:12">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" ht="30" customHeight="1" spans="1:12">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="B16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" ht="30" customHeight="1" spans="1:12">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="B17" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="18" t="s">
+      <c r="I17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" ht="30" customHeight="1"/>
-    <row r="5" ht="30" customHeight="1"/>
-    <row r="6" ht="30" customHeight="1"/>
-    <row r="7" ht="30" customHeight="1"/>
-    <row r="8" ht="30" customHeight="1"/>
-    <row r="9" ht="30" customHeight="1"/>
-    <row r="10" ht="30" customHeight="1"/>
-    <row r="11" ht="30" customHeight="1"/>
-    <row r="12" ht="30" customHeight="1"/>
-    <row r="13" ht="30" customHeight="1"/>
-    <row r="14" ht="30" customHeight="1"/>
-    <row r="15" ht="30" customHeight="1"/>
-    <row r="16" ht="30" customHeight="1"/>
-    <row r="17" ht="30" customHeight="1"/>
     <row r="18" ht="30" customHeight="1"/>
     <row r="19" ht="30" customHeight="1"/>
     <row r="20" ht="30" customHeight="1"/>
@@ -1824,14 +2795,19 @@
     <row r="24" ht="30" customHeight="1"/>
     <row r="25" ht="30" customHeight="1"/>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D12"/>
+    <mergeCell ref="D15:D17"/>
+  </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1 I2:I3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I15 I1:I14 I16:I17">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1 L2:L3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L15 L1:L14 L16:L17">
       <formula1>"Pass,Fail,Hold"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H14 H15:H17">
       <formula1>"GET,POST,PUT,DELETE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1845,8 +2821,8 @@
   <sheetPr/>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1907,34 +2883,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>22</v>
@@ -1945,32 +2921,32 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>22</v>
@@ -1981,29 +2957,29 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="K4" s="18" t="s">
         <v>21</v>
@@ -2017,34 +2993,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>22</v>
@@ -2055,32 +3031,32 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>22</v>
@@ -2091,29 +3067,29 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>21</v>
@@ -2127,34 +3103,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J8" s="16" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>22</v>
@@ -2165,32 +3141,32 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="G9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J9" s="16" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>22</v>
@@ -2201,34 +3177,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="G10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J10" s="16" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>22</v>
@@ -2239,32 +3215,32 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="G11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J11" s="16" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>22</v>
@@ -2275,32 +3251,32 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="G12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J12" s="16" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>22</v>
@@ -2311,32 +3287,32 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J13" s="16" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>22</v>
@@ -2347,32 +3323,32 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="G14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J14" s="16" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>22</v>
@@ -2383,32 +3359,32 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="G15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J15" s="16" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>22</v>
@@ -2419,34 +3395,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="G16" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J16" s="16" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>22</v>
@@ -2457,34 +3433,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="G17" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J17" s="16" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>22</v>
@@ -2495,32 +3471,32 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="G18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J18" s="16" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>22</v>
@@ -2531,34 +3507,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J19" s="16" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>22</v>
@@ -2569,35 +3545,35 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="7" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="G20" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="J20" s="16" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="L20" s="23" t="s">
-        <v>83</v>
+        <v>109</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1" spans="1:12">

</xml_diff>

<commit_message>
Add email verfiy API
</commit_message>
<xml_diff>
--- a/Files/IKSANA_API_TEST_SCRIPTS_v0.1.xlsx
+++ b/Files/IKSANA_API_TEST_SCRIPTS_v0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6080" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="6800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="168">
   <si>
     <t>S.NO</t>
   </si>
@@ -535,6 +535,58 @@
     <t>HTTP status code should be 200 and The response should contain "1111" code and "OTP Expired" message.</t>
   </si>
   <si>
+    <t>Login_TC_17</t>
+  </si>
+  <si>
+    <t>LoginSessionCheck</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Login :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/login-with-otp
+&amp;
+http://135.181.193.65:8080/session-verification</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation for User have another session.</t>
+  </si>
+  <si>
+    <t>session-verification</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>HTTP status code should be 200 and The response should contain "0000" code and "Login Successfully" message.</t>
+  </si>
+  <si>
+    <t>Login_TC_18</t>
+  </si>
+  <si>
+    <t>LoginSessionValidationCheck</t>
+  </si>
+  <si>
+    <t>HTTP status code should be 200 and The response should contain "1111" code and "Enter valid data" message.</t>
+  </si>
+  <si>
     <t>Registration_TC_01</t>
   </si>
   <si>
@@ -573,9 +625,6 @@
     <t>user-registration</t>
   </si>
   <si>
-    <t>POST</t>
-  </si>
-  <si>
     <t>HTTP status code should be 200 OK.</t>
   </si>
   <si>
@@ -724,6 +773,99 @@
   </si>
   <si>
     <t>Verify the API response status and validation of email field upon null values on caregiver.</t>
+  </si>
+  <si>
+    <t>Registration_TC_20</t>
+  </si>
+  <si>
+    <t>userVerificationSuccess</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Email Verification :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://135.181.193.65:8080/rest/api/v1/email-verify
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of Valid user email verification</t>
+  </si>
+  <si>
+    <t>email-verify</t>
+  </si>
+  <si>
+    <t>The response should contain "0000" code and "Successfully created" message</t>
+  </si>
+  <si>
+    <t>Registration_TC_21</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of Valid user phonenumber verification</t>
+  </si>
+  <si>
+    <t>Registration_TC_22</t>
+  </si>
+  <si>
+    <t>userVerificationEmailFailure</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of Invalid email verification</t>
+  </si>
+  <si>
+    <t>The response should contain "1111" code and "Please enter valid email address" message</t>
+  </si>
+  <si>
+    <t>Registration_TC_23</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of Duplicate email verification</t>
+  </si>
+  <si>
+    <t>The response should contain "1111" code and "Email address is already exists" message</t>
+  </si>
+  <si>
+    <t>Registration_TC_24</t>
+  </si>
+  <si>
+    <t>userVerificationPhoneNoFailure</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of Invalid phoneNumber verification</t>
+  </si>
+  <si>
+    <t>The response should contain "1111" code and "Please enter valid contact number" message</t>
+  </si>
+  <si>
+    <t>Registration_TC_25</t>
+  </si>
+  <si>
+    <t>The response should contain "1111" code and "Contact number already exists" message</t>
+  </si>
+  <si>
+    <t>Registration_TC_26</t>
+  </si>
+  <si>
+    <t>Verify the API response status and validation of payload value :"email" and email = null phone number verification</t>
+  </si>
+  <si>
+    <t>The response should contain "1111" code and "Email cannot be null" message</t>
   </si>
 </sst>
 </file>
@@ -736,7 +878,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -782,7 +924,18 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1140,7 +1293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1214,17 +1367,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -1235,6 +1377,26 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1355,137 +1517,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1549,12 +1711,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1570,10 +1750,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1582,14 +1759,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2142,8 +2313,8 @@
   <sheetPr/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -2169,7 +2340,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -2178,7 +2349,7 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="30" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -2239,23 +2410,23 @@
       </c>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:12">
-      <c r="A3" s="25">
+      <c r="A3" s="31">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="31" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="33" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -2264,13 +2435,13 @@
       <c r="I3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="36" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="31" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2281,7 +2452,7 @@
       <c r="B4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -2319,7 +2490,7 @@
       <c r="B5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="5"/>
@@ -2355,7 +2526,7 @@
       <c r="B6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="5"/>
@@ -2391,7 +2562,7 @@
       <c r="B7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="5"/>
@@ -2427,7 +2598,7 @@
       <c r="B8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="5"/>
@@ -2452,7 +2623,7 @@
       <c r="K8" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="28" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2463,7 +2634,7 @@
       <c r="B9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="5"/>
@@ -2488,7 +2659,7 @@
       <c r="K9" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="L9" s="34" t="s">
+      <c r="L9" s="28" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2499,7 +2670,7 @@
       <c r="B10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="5"/>
@@ -2524,7 +2695,7 @@
       <c r="K10" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="34" t="s">
+      <c r="L10" s="28" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2535,7 +2706,7 @@
       <c r="B11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="5"/>
@@ -2560,28 +2731,28 @@
       <c r="K11" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="34" t="s">
+      <c r="L11" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1" spans="1:12">
-      <c r="A12" s="25">
+      <c r="A12" s="31">
         <v>11</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="30" t="s">
+      <c r="D12" s="31"/>
+      <c r="E12" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="33" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="13" t="s">
@@ -2596,7 +2767,7 @@
       <c r="K12" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="25" t="s">
+      <c r="L12" s="31" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2619,7 +2790,7 @@
       <c r="F13" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="23" t="s">
         <v>62</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -2657,7 +2828,7 @@
       <c r="F14" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="23" t="s">
         <v>62</v>
       </c>
       <c r="H14" s="9" t="s">
@@ -2683,19 +2854,19 @@
       <c r="B15" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="22" t="s">
         <v>60</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="23" t="s">
         <v>62</v>
       </c>
       <c r="H15" s="9" t="s">
@@ -2721,17 +2892,17 @@
       <c r="B16" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="22" t="s">
         <v>60</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="23" t="s">
         <v>62</v>
       </c>
       <c r="H16" s="9" t="s">
@@ -2757,17 +2928,17 @@
       <c r="B17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="33" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="22" t="s">
         <v>60</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="23" t="s">
         <v>62</v>
       </c>
       <c r="H17" s="9" t="s">
@@ -2786,8 +2957,82 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" ht="30" customHeight="1"/>
-    <row r="19" ht="30" customHeight="1"/>
+    <row r="18" customFormat="1" ht="30" customHeight="1" spans="1:12">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="1" ht="30" customHeight="1" spans="1:12">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="20" ht="30" customHeight="1"/>
     <row r="21" ht="30" customHeight="1"/>
     <row r="22" ht="30" customHeight="1"/>
@@ -2801,14 +3046,14 @@
     <mergeCell ref="D15:D17"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I15 I1:I14 I16:I17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H17">
+      <formula1>"GET,POST,PUT,DELETE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I17">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L15 L1:L14 L16:L17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L17">
       <formula1>"Pass,Fail,Hold"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H14 H15:H17">
-      <formula1>"GET,POST,PUT,DELETE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2821,8 +3066,8 @@
   <sheetPr/>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -2883,34 +3128,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>86</v>
+        <v>94</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>95</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>22</v>
@@ -2921,32 +3166,32 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>90</v>
+        <v>98</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>99</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>22</v>
@@ -2957,29 +3202,29 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="G4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="K4" s="18" t="s">
         <v>21</v>
@@ -2993,34 +3238,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="G5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>86</v>
+        <v>94</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>95</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>22</v>
@@ -3031,32 +3276,32 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="G6" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="K6" s="22" t="s">
-        <v>90</v>
+        <v>98</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>99</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>22</v>
@@ -3067,29 +3312,29 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="G7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>21</v>
@@ -3103,34 +3348,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>22</v>
@@ -3141,32 +3386,32 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="G9" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>22</v>
@@ -3177,34 +3422,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="G10" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>22</v>
@@ -3215,32 +3460,32 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="G11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>22</v>
@@ -3251,32 +3496,32 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="G12" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>22</v>
@@ -3287,32 +3532,32 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>22</v>
@@ -3323,32 +3568,32 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="G14" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>22</v>
@@ -3359,32 +3604,32 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="G15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>22</v>
@@ -3395,34 +3640,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="G16" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>22</v>
@@ -3433,34 +3678,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>22</v>
@@ -3471,32 +3716,32 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="G18" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>22</v>
@@ -3507,34 +3752,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>22</v>
@@ -3545,179 +3790,342 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="7" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="G20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>30</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" ht="30" customHeight="1" spans="1:12">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" ht="30" customHeight="1" spans="1:12">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" ht="30" customHeight="1" spans="1:12">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="5"/>
-    </row>
-    <row r="24" ht="30" customHeight="1" spans="1:12">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="5"/>
-    </row>
-    <row r="25" ht="30" customHeight="1" spans="1:12">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="5"/>
-    </row>
-    <row r="26" ht="30" customHeight="1" spans="1:12">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="5"/>
-    </row>
-    <row r="27" ht="30" customHeight="1" spans="1:12">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="5"/>
+    <row r="21" customFormat="1" ht="30" customHeight="1" spans="1:12">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" customFormat="1" ht="30" customHeight="1" spans="1:12">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customFormat="1" ht="30" customHeight="1" spans="1:12">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="1" ht="30" customHeight="1" spans="1:12">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" customFormat="1" ht="30" customHeight="1" spans="1:12">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customFormat="1" ht="30" customHeight="1" spans="1:12">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="26"/>
+      <c r="E26" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" customFormat="1" ht="30" customHeight="1" spans="1:12">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="L27" s="28" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:12">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
       <c r="L28" s="5"/>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:12">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
       <c r="L29" s="5"/>
     </row>
     <row r="30" ht="30" customHeight="1" spans="7:12">
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
       <c r="L30" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D10:D15"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D25:D27"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H20">

</xml_diff>